<commit_message>
compute critical path and some changes in circuit dictionary and create critical path xlsx file.
</commit_message>
<xml_diff>
--- a/Outputs/For Test/AND.xlsx
+++ b/Outputs/For Test/AND.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
-  <si>
-    <t>Benchmark AND Vulnerability Factor</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+  <si>
+    <t>Benchmark For Test/AND Vulnerability Factor</t>
   </si>
   <si>
     <t>Types</t>
@@ -34,31 +34,16 @@
     <t>Vulnerability Factors (VF)</t>
   </si>
   <si>
-    <t>Gate Inputs List</t>
+    <t>Gate Delay</t>
   </si>
   <si>
     <t>PI</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>AND</t>
   </si>
   <si>
-    <t>['1', '2']</t>
-  </si>
-  <si>
-    <t>['4', '5']</t>
-  </si>
-  <si>
-    <t>['8', '9']</t>
-  </si>
-  <si>
     <t>AND(PO)</t>
-  </si>
-  <si>
-    <t>['6', '3', '7']</t>
   </si>
 </sst>
 </file>
@@ -503,8 +488,8 @@
       <c r="E3" s="3">
         <v>0</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
+      <c r="F3" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -523,8 +508,8 @@
       <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
+      <c r="F4" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -543,8 +528,8 @@
       <c r="E5" s="3">
         <v>0</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>8</v>
+      <c r="F5" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -563,8 +548,8 @@
       <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>8</v>
+      <c r="F6" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -583,8 +568,8 @@
       <c r="E7" s="3">
         <v>0</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>8</v>
+      <c r="F7" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -603,13 +588,13 @@
       <c r="E8" s="3">
         <v>0</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>8</v>
+      <c r="F8" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3">
         <v>3</v>
@@ -623,13 +608,13 @@
       <c r="E9" s="3">
         <v>0.5</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>10</v>
+      <c r="F9" s="3">
+        <v>19.8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>6</v>
@@ -643,13 +628,13 @@
       <c r="E10" s="3">
         <v>0.5</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>11</v>
+      <c r="F10" s="3">
+        <v>19.8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3">
         <v>7</v>
@@ -663,13 +648,13 @@
       <c r="E11" s="3">
         <v>0.5</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>12</v>
+      <c r="F11" s="3">
+        <v>19.8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3">
         <v>10</v>
@@ -683,8 +668,8 @@
       <c r="E12" s="3">
         <v>0.96875</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>14</v>
+      <c r="F12" s="3">
+        <v>39.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>